<commit_message>
primera edición tema 4
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion04/SolicitudGrafica_MA_04_04_CO_REC10.xlsx
+++ b/fuentes/contenidos/grado04/guion04/SolicitudGrafica_MA_04_04_CO_REC10.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="159">
   <si>
     <t>Asignatura:</t>
   </si>
@@ -545,6 +545,12 @@
   <si>
     <t>IMG03</t>
   </si>
+  <si>
+    <t>Niño leyendo un libro</t>
+  </si>
+  <si>
+    <t>Grupo de galletas de chips de chocolate</t>
+  </si>
 </sst>
 </file>
 
@@ -553,7 +559,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -596,16 +602,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Century Gothic"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
     </font>
     <font>
@@ -910,21 +906,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1195,6 +1176,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1249,7 +1243,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1295,45 +1289,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1351,70 +1336,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1426,46 +1420,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1486,38 +1480,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1537,20 +1531,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1684,6 +1673,231 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1103313</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>55562</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4396827</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2708671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Oranges isolated cut set on wooden base"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17462501" y="2008187"/>
+          <a:ext cx="3293514" cy="2653109"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1270000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>39688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4146443</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>3525838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="Group of teen school child with book.  Isolated."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17629188" y="4786313"/>
+          <a:ext cx="2876443" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1309688</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>87313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4360804</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>2263776</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Child opened a magic book"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17668876" y="8509001"/>
+          <a:ext cx="3051116" cy="2176463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4984750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>3119438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5" descr="Oatmeal cookies with wooden background."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17057688" y="10779126"/>
+          <a:ext cx="4286250" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -2398,9 +2612,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14:E15"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2428,8 +2642,8 @@
       <c r="D1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
@@ -2446,8 +2660,8 @@
         <v>1</v>
       </c>
       <c r="G2" s="76"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2461,8 +2675,8 @@
       <c r="D3" s="85"/>
       <c r="F3" s="77"/>
       <c r="G3" s="78"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
       <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
@@ -2475,14 +2689,14 @@
       </c>
       <c r="D4" s="85"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
@@ -2496,15 +2710,15 @@
       </c>
       <c r="D5" s="87"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="48" t="str">
+      <c r="F5" s="45" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
         <v>Motor del recurso</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="72"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="69"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
@@ -2516,20 +2730,20 @@
       <c r="E6" s="7"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="31" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="1"/>
@@ -2560,52 +2774,52 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="I9" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="107" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="74">
+      <c r="B10" s="71">
         <v>156930275</v>
       </c>
-      <c r="C10" s="27" t="str">
+      <c r="C10" s="25" t="str">
         <f t="shared" ref="C10:C14" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F1</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="72" t="s">
         <v>152</v>
       </c>
       <c r="E10" s="14" t="s">
@@ -2627,19 +2841,19 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J10" s="107" t="s">
+      <c r="J10" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="K10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.3">
-      <c r="A11" s="108" t="s">
+      <c r="K10" s="106"/>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="290.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="B11" s="74">
+      <c r="B11" s="71">
         <v>113607577</v>
       </c>
-      <c r="C11" s="27" t="str">
+      <c r="C11" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F1</v>
       </c>
@@ -2665,23 +2879,23 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J11" s="107" t="s">
+      <c r="J11" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="108" t="s">
+      <c r="K11" s="106"/>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="71">
         <v>175520738</v>
       </c>
-      <c r="C12" s="27" t="str">
+      <c r="C12" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F1</v>
       </c>
-      <c r="D12" s="106" t="s">
+      <c r="D12" s="72" t="s">
         <v>152</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -2703,21 +2917,24 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="21"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="249.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="71">
         <v>179788793</v>
       </c>
-      <c r="C13" s="27" t="str">
+      <c r="C13" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F1</v>
       </c>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="72" t="s">
         <v>152</v>
       </c>
       <c r="E13" s="14" t="s">
@@ -2739,16 +2956,18 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="21"/>
+      <c r="J13" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="K13" s="106"/>
     </row>
     <row r="14" spans="1:16" s="12" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="str">
-        <f t="shared" ref="A11:A22" si="3">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(LEFT(A13,3),IF(MID(A13,4,2)+1&lt;10,CONCATENATE("0",MID(A13,4,2)+1))),"")</f>
-        <v/>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="27" t="str">
+        <f t="shared" ref="A14:A22" si="3">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(LEFT(A13,3),IF(MID(A13,4,2)+1&lt;10,CONCATENATE("0",MID(A13,4,2)+1))),"")</f>
+        <v/>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2778,8 +2997,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="27" t="str">
+      <c r="B15" s="26"/>
+      <c r="C15" s="25" t="str">
         <f t="shared" ref="C15" si="4">IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
@@ -2809,8 +3028,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14" t="str">
@@ -2837,8 +3056,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="14" t="str">
@@ -2865,8 +3084,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="14" t="str">
@@ -2893,8 +3112,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="14" t="str">
@@ -2921,8 +3140,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14" t="str">
@@ -2949,8 +3168,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14" t="str">
@@ -2977,8 +3196,8 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14" t="str">
@@ -3002,8 +3221,8 @@
     </row>
     <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="str">
@@ -3027,8 +3246,8 @@
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14" t="str">
@@ -3052,8 +3271,8 @@
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14" t="str">
@@ -3077,8 +3296,8 @@
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14" t="str">
@@ -3102,8 +3321,8 @@
     </row>
     <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="14" t="str">
@@ -3127,8 +3346,8 @@
     </row>
     <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14" t="str">
@@ -3152,8 +3371,8 @@
     </row>
     <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14" t="str">
@@ -3172,13 +3391,13 @@
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J29" s="22"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14" t="str">
@@ -3197,13 +3416,13 @@
         <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J30" s="23"/>
+      <c r="J30" s="22"/>
       <c r="K30" s="15"/>
     </row>
     <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14" t="str">
@@ -3227,8 +3446,8 @@
     </row>
     <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14" t="str">
@@ -3252,8 +3471,8 @@
     </row>
     <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="14" t="str">
@@ -3277,8 +3496,8 @@
     </row>
     <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="14" t="str">
@@ -3302,8 +3521,8 @@
     </row>
     <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="14" t="str">
@@ -3327,8 +3546,8 @@
     </row>
     <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="14" t="str">
@@ -3352,8 +3571,8 @@
     </row>
     <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14" t="str">
@@ -3377,8 +3596,8 @@
     </row>
     <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14" t="str">
@@ -3402,8 +3621,8 @@
     </row>
     <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14" t="str">
@@ -3427,8 +3646,8 @@
     </row>
     <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="14" t="str">
@@ -3452,8 +3671,8 @@
     </row>
     <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14" t="str">
@@ -3477,8 +3696,8 @@
     </row>
     <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="str">
@@ -3502,8 +3721,8 @@
     </row>
     <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="14" t="str">
@@ -3527,8 +3746,8 @@
     </row>
     <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="14" t="str">
@@ -3552,8 +3771,8 @@
     </row>
     <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="14" t="str">
@@ -3577,8 +3796,8 @@
     </row>
     <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14" t="str">
@@ -3602,8 +3821,8 @@
     </row>
     <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="14" t="str">
@@ -3627,8 +3846,8 @@
     </row>
     <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14" t="str">
@@ -3652,8 +3871,8 @@
     </row>
     <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="14" t="str">
@@ -3677,8 +3896,8 @@
     </row>
     <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14" t="str">
@@ -3702,8 +3921,8 @@
     </row>
     <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="14" t="str">
@@ -3727,8 +3946,8 @@
     </row>
     <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="14" t="str">
@@ -3752,8 +3971,8 @@
     </row>
     <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="14" t="str">
@@ -4999,6 +5218,7 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5018,13 +5238,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="33" customWidth="1"/>
-    <col min="2" max="2" width="11" style="33"/>
-    <col min="3" max="3" width="13.875" style="33" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="33" customWidth="1"/>
-    <col min="5" max="7" width="11" style="33"/>
-    <col min="8" max="11" width="11" style="33" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="33"/>
+    <col min="1" max="1" width="72.25" style="30" customWidth="1"/>
+    <col min="2" max="2" width="11" style="30"/>
+    <col min="3" max="3" width="13.875" style="30" customWidth="1"/>
+    <col min="4" max="4" width="11.375" style="30" customWidth="1"/>
+    <col min="5" max="7" width="11" style="30"/>
+    <col min="8" max="11" width="11" style="30" hidden="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5038,75 +5258,75 @@
       <c r="F1" s="92"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="93" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="94"/>
       <c r="E2" s="95"/>
-      <c r="F2" s="43"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="99" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="100"/>
       <c r="E3" s="101"/>
-      <c r="F3" s="43"/>
-      <c r="H3" s="33" t="s">
+      <c r="F3" s="40"/>
+      <c r="H3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="H4" s="33" t="s">
+      <c r="F4" s="40"/>
+      <c r="H4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="30">
         <v>1</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="39" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="36" t="s">
         <v>36</v>
       </c>
       <c r="D5" s="102" t="str">
@@ -5114,48 +5334,48 @@
         <v>LE_07_04_CO</v>
       </c>
       <c r="E5" s="103"/>
-      <c r="F5" s="43"/>
-      <c r="H5" s="33" t="s">
+      <c r="F5" s="40"/>
+      <c r="H5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="30">
         <v>2</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="H6" s="33" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="H6" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="30">
         <v>3</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="70" t="s">
         <v>144</v>
       </c>
       <c r="D7" s="88" t="str">
@@ -5164,95 +5384,95 @@
       </c>
       <c r="E7" s="88"/>
       <c r="F7" s="89"/>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="30">
         <v>4</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="30">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="I8" s="33" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="I8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="30">
         <v>5</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="I9" s="33" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="I9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="30">
         <v>6</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="30">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
-      <c r="I10" s="33" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="I10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="30">
         <v>7</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="30">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="30">
         <v>8</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="30">
         <v>9</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="30">
         <v>9</v>
       </c>
     </row>
@@ -5265,81 +5485,81 @@
       <c r="D13" s="91"/>
       <c r="E13" s="91"/>
       <c r="F13" s="92"/>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="33">
+      <c r="J13" s="30">
         <v>10</v>
       </c>
-      <c r="K13" s="33">
+      <c r="K13" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="I14" s="33" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+      <c r="I14" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="30">
         <v>11</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="30">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="42"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="93" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="94"/>
       <c r="E15" s="94"/>
       <c r="F15" s="95"/>
-      <c r="J15" s="33">
+      <c r="J15" s="30">
         <v>12</v>
       </c>
-      <c r="K15" s="33">
+      <c r="K15" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="30">
         <v>13</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="30">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="39" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="96" t="str">
@@ -5348,19 +5568,19 @@
       </c>
       <c r="E17" s="97"/>
       <c r="F17" s="98"/>
-      <c r="J17" s="33">
+      <c r="J17" s="30">
         <v>14</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="30">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="73" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="70" t="s">
         <v>145</v>
       </c>
       <c r="D18" s="88" t="str">
@@ -5369,188 +5589,188 @@
       </c>
       <c r="E18" s="88"/>
       <c r="F18" s="89"/>
-      <c r="J18" s="33">
+      <c r="J18" s="30">
         <v>15</v>
       </c>
-      <c r="K18" s="33">
+      <c r="K18" s="30">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="H19" s="33">
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
+      <c r="H19" s="30">
         <v>3</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="30">
         <v>16</v>
       </c>
-      <c r="K19" s="33">
+      <c r="K19" s="30">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47"/>
-      <c r="H20" s="33">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="H20" s="30">
         <v>4</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="30">
         <v>5</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="30">
         <v>4</v>
       </c>
-      <c r="K20" s="33">
+      <c r="K20" s="30">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H21" s="33" t="str">
+      <c r="H21" s="30" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
       </c>
-      <c r="I21" s="33" t="str">
+      <c r="I21" s="30" t="str">
         <f>CONCATENATE(IF((I20+2)&lt;10,"0",""),I20+2)</f>
         <v>07</v>
       </c>
-      <c r="J21" s="33" t="str">
+      <c r="J21" s="30" t="str">
         <f>CONCATENATE(IF(J20&lt;10,"0",""),J20)</f>
         <v>04</v>
       </c>
-      <c r="K21" s="33">
+      <c r="K21" s="30">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K22" s="33">
+      <c r="K22" s="30">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="33">
+      <c r="K23" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K24" s="33">
+      <c r="K24" s="30">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="33">
+      <c r="K25" s="30">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="33">
+      <c r="K26" s="30">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K27" s="33">
+      <c r="K27" s="30">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K28" s="33">
+      <c r="K28" s="30">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K29" s="33">
+      <c r="K29" s="30">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K30" s="33">
+      <c r="K30" s="30">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K31" s="33">
+      <c r="K31" s="30">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K32" s="33">
+      <c r="K32" s="30">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="33">
+      <c r="K33" s="30">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34" s="33">
+      <c r="K34" s="30">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35" s="33">
+      <c r="K35" s="30">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36" s="33">
+      <c r="K36" s="30">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K37" s="33">
+      <c r="K37" s="30">
         <v>34</v>
       </c>
     </row>
     <row r="38" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K38" s="33">
+      <c r="K38" s="30">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K39" s="33">
+      <c r="K39" s="30">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K40" s="33">
+      <c r="K40" s="30">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K41" s="33">
+      <c r="K41" s="30">
         <v>38</v>
       </c>
     </row>
     <row r="42" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K42" s="33">
+      <c r="K42" s="30">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K43" s="33">
+      <c r="K43" s="30">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K44" s="33">
+      <c r="K44" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K45" s="33" t="str">
+      <c r="K45" s="30" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
       </c>
@@ -5745,17 +5965,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="33" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="33" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="33" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="33"/>
-    <col min="5" max="5" width="11.75" style="33" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="33" customWidth="1"/>
-    <col min="7" max="7" width="11" style="33" customWidth="1"/>
-    <col min="8" max="9" width="22.25" style="33" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="33" customWidth="1"/>
-    <col min="11" max="11" width="44.5" style="33" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="33"/>
+    <col min="1" max="1" width="21" style="30" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="30"/>
+    <col min="5" max="5" width="11.75" style="30" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="30" customWidth="1"/>
+    <col min="7" max="7" width="11" style="30" customWidth="1"/>
+    <col min="8" max="9" width="22.25" style="30" customWidth="1"/>
+    <col min="10" max="10" width="20.75" style="30" customWidth="1"/>
+    <col min="11" max="11" width="44.5" style="30" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -5794,510 +6014,510 @@
       <c r="E2" s="104"/>
       <c r="F2" s="104"/>
       <c r="G2" s="104"/>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="49" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53" t="s">
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-    </row>
-    <row r="4" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+    </row>
+    <row r="4" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55" t="s">
+      <c r="G4" s="52"/>
+      <c r="H4" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="55"/>
-    </row>
-    <row r="5" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="J4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="57"/>
-      <c r="H5" s="55" t="s">
+      <c r="G5" s="54"/>
+      <c r="H5" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="57"/>
-    </row>
-    <row r="6" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="J5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="55" t="s">
+      <c r="J6" s="52" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="54" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+    <row r="7" spans="1:11" s="51" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="55"/>
-    </row>
-    <row r="8" spans="1:11" s="54" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="J7" s="52"/>
+    </row>
+    <row r="8" spans="1:11" s="51" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55" t="s">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="55"/>
-    </row>
-    <row r="9" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="s">
+      <c r="J8" s="52"/>
+    </row>
+    <row r="9" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55" t="s">
+      <c r="G9" s="52"/>
+      <c r="H9" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="55"/>
-    </row>
-    <row r="10" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="J9" s="52"/>
+    </row>
+    <row r="10" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55" t="s">
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-    </row>
-    <row r="11" spans="1:11" s="54" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="s">
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+    </row>
+    <row r="11" spans="1:11" s="51" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="55" t="s">
+      <c r="D11" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55" t="s">
+      <c r="G11" s="52"/>
+      <c r="H11" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="55" t="s">
+      <c r="I11" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="55"/>
-    </row>
-    <row r="12" spans="1:11" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55" t="s">
+      <c r="G12" s="52"/>
+      <c r="H12" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="55" t="s">
+      <c r="I12" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60" t="s">
+      <c r="E13" s="56"/>
+      <c r="F13" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55" t="s">
+      <c r="G13" s="55"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="33" t="s">
+      <c r="J13" s="55"/>
+      <c r="K13" s="30" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60" t="s">
+      <c r="E14" s="56"/>
+      <c r="F14" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55" t="s">
+      <c r="G14" s="55"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="58"/>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="55" t="s">
         <v>141</v>
       </c>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="55" t="s">
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="33" t="s">
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="56" t="s">
+      <c r="B16" s="57"/>
+      <c r="C16" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="59"/>
-      <c r="H16" s="60" t="s">
+      <c r="G16" s="56"/>
+      <c r="H16" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="I16" s="60" t="s">
+      <c r="I16" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="J16" s="59"/>
-      <c r="K16" s="61" t="s">
+      <c r="J16" s="56"/>
+      <c r="K16" s="58" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55" t="s">
+      <c r="B17" s="52"/>
+      <c r="C17" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="G17" s="55"/>
-      <c r="H17" s="62" t="s">
+      <c r="G17" s="52"/>
+      <c r="H17" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="62" t="s">
+      <c r="I17" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="J17" s="55"/>
-      <c r="K17" s="63" t="s">
+      <c r="J17" s="52"/>
+      <c r="K17" s="60" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="61" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B22" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="69" t="s">
+      <c r="B23" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
     </row>
     <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="65" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="69" t="s">
+      <c r="B25" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="70" t="s">
+      <c r="C25" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
     </row>
     <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B26" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>